<commit_message>
Updated the code to Read Data from the Excel Sheet
Updated the code to Read Data from the Excel Sheet
</commit_message>
<xml_diff>
--- a/Resources/TestData_Input.xlsx
+++ b/Resources/TestData_Input.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakir\eclipse-workspace\Automation_Selenium_TestNG\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D7A8F9-124A-4C11-8192-AAA8521A47C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB10354-1725-4BC4-9882-BF2802AA517A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F82B3574-0BB9-4FA9-B954-18378FCFCBB7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F82B3574-0BB9-4FA9-B954-18378FCFCBB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
     <sheet name="PIM" sheetId="2" r:id="rId2"/>
+    <sheet name="TIME" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,18 +27,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="17">
   <si>
     <t>userName</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>Time_TestCase01</t>
+  </si>
+  <si>
+    <t>passWord</t>
+  </si>
+  <si>
+    <t>searchUser</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>zakir</t>
+  </si>
+  <si>
+    <t>PIM_TestCase01</t>
+  </si>
+  <si>
+    <t>Admin_TestCase01</t>
+  </si>
+  <si>
+    <t>empName</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>erere</t>
+  </si>
+  <si>
+    <t>ere</t>
+  </si>
+  <si>
+    <t>eress</t>
   </si>
 </sst>
 </file>
@@ -53,15 +93,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -69,12 +115,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,43 +466,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CFE993-A339-4F88-BF81-48A7280F5EA0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA78D0B-597B-4727-B4EB-994E7F96AF7E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E7222F-4E1B-44E5-8EC2-2D90E6A337A7}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Code to read data from Excel Sheet
</commit_message>
<xml_diff>
--- a/Resources/TestData_Input.xlsx
+++ b/Resources/TestData_Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakir\eclipse-workspace\Automation_Selenium_TestNG\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blues\git\Automation_Selenium_TestNG\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB10354-1725-4BC4-9882-BF2802AA517A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856575CC-5F07-4827-A0EB-6B3F043F7797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F82B3574-0BB9-4FA9-B954-18378FCFCBB7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F82B3574-0BB9-4FA9-B954-18378FCFCBB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>userName</t>
   </si>
@@ -53,21 +53,9 @@
     <t>PIM_TestCase01</t>
   </si>
   <si>
-    <t>Admin_TestCase01</t>
-  </si>
-  <si>
     <t>empName</t>
   </si>
   <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -78,6 +66,54 @@
   </si>
   <si>
     <t>eress</t>
+  </si>
+  <si>
+    <t>Time_TestCase02</t>
+  </si>
+  <si>
+    <t>Time_TestCase03</t>
+  </si>
+  <si>
+    <t>Time_TestCase04</t>
+  </si>
+  <si>
+    <t>Admin_TC01</t>
+  </si>
+  <si>
+    <t>loginUser</t>
+  </si>
+  <si>
+    <t>loginPassWord</t>
+  </si>
+  <si>
+    <t>userRole</t>
+  </si>
+  <si>
+    <t>newUserPassWord</t>
+  </si>
+  <si>
+    <t>newUserConfirmPassWord</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>zakir_qa</t>
+  </si>
+  <si>
+    <t>rules123</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Admin_TC02</t>
+  </si>
+  <si>
+    <t>loginPassword</t>
+  </si>
+  <si>
+    <t>Lokesh</t>
   </si>
 </sst>
 </file>
@@ -147,11 +183,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,39 +503,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CFE993-A339-4F88-BF81-48A7280F5EA0}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
@@ -506,7 +563,50 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -519,16 +619,16 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -545,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
@@ -565,24 +665,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E7222F-4E1B-44E5-8EC2-2D90E6A337A7}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -591,13 +691,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
@@ -608,9 +708,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -619,13 +719,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -636,9 +736,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
@@ -647,19 +747,19 @@
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -670,15 +770,15 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
@@ -687,13 +787,13 @@
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Listners and Extend Reports
</commit_message>
<xml_diff>
--- a/Resources/TestData_Input.xlsx
+++ b/Resources/TestData_Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blues\git\Automation_Selenium_TestNG\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakir\eclipse-workspace\Automation_Selenium_TestNG\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856575CC-5F07-4827-A0EB-6B3F043F7797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A874A394-38D0-4D66-AC94-B61E127FF452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F82B3574-0BB9-4FA9-B954-18378FCFCBB7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F82B3574-0BB9-4FA9-B954-18378FCFCBB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -506,24 +506,24 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -555,7 +555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
@@ -581,7 +581,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -598,7 +598,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -622,13 +622,13 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -645,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
@@ -669,18 +669,18 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -697,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
@@ -708,7 +708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -725,7 +725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -736,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -759,7 +759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -776,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -793,7 +793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>